<commit_message>
Correct bug in cMessageLogger
</commit_message>
<xml_diff>
--- a/Examples/ecos25/Cloralkali.xlsx
+++ b/Examples/ecos25/Cloralkali.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\cgam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\ecos25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A0C5D7-8045-4F5D-9D0D-AFCFC7C6AB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2968CE8-6D1B-43A7-BB9A-0ACE255B92CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27840" windowHeight="14325" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="3" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="Exergy" sheetId="7" r:id="rId5"/>
     <sheet name="Format" sheetId="8" r:id="rId6"/>
     <sheet name="WasteDefinition" sheetId="9" r:id="rId7"/>
-    <sheet name="ResourcesCost" sheetId="10" r:id="rId8"/>
-    <sheet name="Balance mat energ" sheetId="1" r:id="rId9"/>
-    <sheet name="Exergías" sheetId="2" r:id="rId10"/>
+    <sheet name="WasteAllocation" sheetId="11" r:id="rId8"/>
+    <sheet name="ResourcesCost" sheetId="10" r:id="rId9"/>
+    <sheet name="Balance mat energ" sheetId="1" r:id="rId10"/>
+    <sheet name="Exergías" sheetId="2" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="tgas_fmt" localSheetId="5">Format!$A$1:$D$7</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="123">
   <si>
     <t>Cl2(g)</t>
   </si>
@@ -254,9 +255,6 @@
     <t>B14</t>
   </si>
   <si>
-    <t>B15</t>
-  </si>
-  <si>
     <t>B16</t>
   </si>
   <si>
@@ -273,18 +271,6 @@
   </si>
   <si>
     <t>B21</t>
-  </si>
-  <si>
-    <t>B22</t>
-  </si>
-  <si>
-    <t>B23</t>
-  </si>
-  <si>
-    <t>B24</t>
-  </si>
-  <si>
-    <t>B25</t>
   </si>
   <si>
     <t>description</t>
@@ -368,9 +354,6 @@
     <t>Purificación Cloro</t>
   </si>
   <si>
-    <t>Purificación Soda</t>
-  </si>
-  <si>
     <t>Desague minería</t>
   </si>
   <si>
@@ -378,9 +361,6 @@
   </si>
   <si>
     <t>Desague salmuera</t>
-  </si>
-  <si>
-    <t>Vapor gastado</t>
   </si>
   <si>
     <t>Sulfurico acuoso</t>
@@ -413,16 +393,46 @@
     <t>B13+B14+B19</t>
   </si>
   <si>
-    <t>B4+B5</t>
+    <t>Cl2</t>
   </si>
   <si>
-    <t>B7+B9</t>
+    <t>H2</t>
   </si>
   <si>
-    <t>B20+B21</t>
+    <t>R22</t>
   </si>
   <si>
-    <t>B12+B16-B17</t>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>B1+B3+(B2-B4-B6)</t>
+  </si>
+  <si>
+    <t>B5+B8+(B6-B7-B10)</t>
+  </si>
+  <si>
+    <t>B12+B13+H2</t>
+  </si>
+  <si>
+    <t>B9+B11+(B10-B14)</t>
+  </si>
+  <si>
+    <t>B13+B14+(B19-B20)</t>
+  </si>
+  <si>
+    <t>Purificación Sosa</t>
+  </si>
+  <si>
+    <t>Vapor Exhaustado</t>
+  </si>
+  <si>
+    <t>B17+NaOH</t>
   </si>
 </sst>
 </file>
@@ -3712,13 +3722,13 @@
   <sheetData>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
       </c>
       <c r="H37" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I37" t="s">
         <v>57</v>
@@ -3726,24 +3736,24 @@
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="O38" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="U38" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="V38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="O43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3753,6 +3763,569 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AD30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="16">
+        <v>244</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="16">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="T1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="17">
+        <f>L2*1000*VLOOKUP(K2,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K2,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>4.6981132075471699</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2">
+        <v>23</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="19">
+        <f>Z2*VLOOKUP(Y2,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(Y2,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>38.3098878695209</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="17">
+        <f>L3*1000*VLOOKUP(K3,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K3,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>5.43025</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1">
+        <f>0.028*0.32</f>
+        <v>8.9600000000000009E-3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="17">
+        <f>L4*1000*VLOOKUP(K4,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K4,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>20.74301369863014</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="16">
+        <v>432</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="16">
+        <f>1787496/1000</f>
+        <v>1787.4960000000001</v>
+      </c>
+      <c r="V5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="16">
+        <f>B7*1000*VLOOKUP(A7,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(A7,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>490.06863449691997</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="16">
+        <f>H7*1000*VLOOKUP(G7,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(G7,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>490.06863449691997</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <f>0.911*1.94</f>
+        <v>1.7673399999999999</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>0.867*2.31</f>
+        <v>2.0027699999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f>0.867*2.31</f>
+        <v>2.0027699999999999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA7">
+        <v>28</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8">
+        <f>2.02+O6*3</f>
+        <v>7.3220200000000002</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <f>7.24/91.4*1000</f>
+        <v>79.212253829321668</v>
+      </c>
+      <c r="V8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <f>O8+L13/1000</f>
+        <v>7.8830200000000001</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="16">
+        <f>28563/1000</f>
+        <v>28.562999999999999</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
+        <v>24</v>
+      </c>
+      <c r="U10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="16">
+        <f>B9*1000*VLOOKUP(A9,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(A7,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>12.012320328542096</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>561</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="17">
+        <f>1231383/1000</f>
+        <v>1231.383</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S14">
+        <f>S13*2</f>
+        <v>2.2559999999999998</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W14" s="16">
+        <f>W15*VLOOKUP(V15,Exergías!$A$1:$C$9,2,FALSE)/VLOOKUP(V15,Exergías!$A$1:$C$9,3,FALSE)</f>
+        <v>3364.4249999999997</v>
+      </c>
+      <c r="X14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <v>28.5</v>
+      </c>
+      <c r="X15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="17">
+        <f>AA15*1000*VLOOKUP(Z15,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(Z15,Exergías!$A$1:$C$8,3,FALSE)</f>
+        <v>1743.3004231311704</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="T18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" t="s">
+        <v>14</v>
+      </c>
+      <c r="T19" t="s">
+        <v>2</v>
+      </c>
+      <c r="U19">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="V19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>0.8</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>8</v>
+      </c>
+      <c r="U20">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="V20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="AA21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB21" s="1">
+        <f>U22+W14+AC15</f>
+        <v>6302.2324231311704</v>
+      </c>
+    </row>
+    <row r="22" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="18">
+        <v>712.15700000000004</v>
+      </c>
+      <c r="P22" t="s">
+        <v>17</v>
+      </c>
+      <c r="T22" t="s">
+        <v>24</v>
+      </c>
+      <c r="U22" s="17">
+        <f>1194507/1000</f>
+        <v>1194.5070000000001</v>
+      </c>
+      <c r="V22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>12</v>
+      </c>
+      <c r="S25">
+        <f>S14-U20</f>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="T25" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="19">
+        <v>611</v>
+      </c>
+      <c r="V25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="R27" t="s">
+        <v>8</v>
+      </c>
+      <c r="S27">
+        <v>0.7</v>
+      </c>
+      <c r="T27" t="s">
+        <v>1</v>
+      </c>
+      <c r="U27" s="16">
+        <v>126.2</v>
+      </c>
+      <c r="V27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="R28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="14:28" x14ac:dyDescent="0.25">
+      <c r="O30" s="1">
+        <f>O22+P13</f>
+        <v>1943.54</v>
+      </c>
+      <c r="P30">
+        <f>U25+U27+U22</f>
+        <v>1931.7070000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="P6">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EDC1F62B-33C6-4008-932E-86963BF76F55}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EDC1F62B-33C6-4008-932E-86963BF76F55}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P6</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -3964,7 +4537,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4091,7 +4664,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>40</v>
@@ -4099,7 +4672,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>32</v>
@@ -4107,7 +4680,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>36</v>
@@ -4115,7 +4688,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -4123,7 +4696,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>32</v>
@@ -4131,7 +4704,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>36</v>
@@ -4139,7 +4712,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>40</v>
@@ -4147,7 +4720,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
@@ -4155,7 +4728,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
@@ -4163,7 +4736,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>42</v>
@@ -4171,7 +4744,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>42</v>
@@ -4253,10 +4826,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="6" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
@@ -4265,183 +4838,183 @@
         <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>70</v>
+      <c r="C7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>71</v>
+      <c r="C8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>72</v>
+        <v>113</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>73</v>
+        <v>114</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
   </sheetData>
@@ -4454,12 +5027,12 @@
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="6" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11.42578125" style="6"/>
   </cols>
@@ -4469,68 +5042,76 @@
         <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>49</v>
+      <c r="A2" s="6" t="str">
+        <f>Flows!A2</f>
+        <v>B1</v>
       </c>
       <c r="B2" s="20">
         <v>490.07859999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>50</v>
+      <c r="A3" s="6" t="str">
+        <f>Flows!A3</f>
+        <v>B2</v>
       </c>
       <c r="B3" s="20">
         <v>12.012320000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>51</v>
+      <c r="A4" s="6" t="str">
+        <f>Flows!A4</f>
+        <v>B3</v>
       </c>
       <c r="B4" s="20">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>52</v>
+      <c r="A5" s="6" t="str">
+        <f>Flows!A5</f>
+        <v>B4</v>
       </c>
       <c r="B5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>53</v>
+      <c r="A6" s="6" t="str">
+        <f>Flows!A6</f>
+        <v>B5</v>
       </c>
       <c r="B6" s="20">
         <v>490.0686</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>54</v>
+      <c r="A7" s="6" t="str">
+        <f>Flows!A7</f>
+        <v>B6</v>
       </c>
       <c r="B7" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>55</v>
+      <c r="A8" s="6" t="str">
+        <f>Flows!A8</f>
+        <v>B7</v>
       </c>
       <c r="B8" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
+      <c r="A9" s="6" t="str">
+        <f>Flows!A9</f>
+        <v>B8</v>
       </c>
       <c r="B9" s="20">
         <f>4.7+5.43+20.7</f>
@@ -4538,72 +5119,81 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>57</v>
+      <c r="A10" s="6" t="str">
+        <f>Flows!A10</f>
+        <v>B9</v>
       </c>
       <c r="B10" s="20">
         <v>432</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>58</v>
+      <c r="A11" s="6" t="str">
+        <f>Flows!A11</f>
+        <v>B10</v>
       </c>
       <c r="B11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>59</v>
+      <c r="A12" s="6" t="str">
+        <f>Flows!A12</f>
+        <v>B11</v>
       </c>
       <c r="B12" s="20">
         <v>20400</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>60</v>
+      <c r="A13" s="6" t="str">
+        <f>Flows!A13</f>
+        <v>B12</v>
       </c>
       <c r="B13" s="20">
         <v>1230</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>61</v>
+      <c r="A14" s="6" t="str">
+        <f>Flows!A14</f>
+        <v>B13</v>
       </c>
       <c r="B14" s="20">
         <v>1787.4960000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>62</v>
+      <c r="A15" s="6" t="str">
+        <f>Flows!A15</f>
+        <v>B14</v>
       </c>
       <c r="B15" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>63</v>
+      <c r="A16" s="6" t="str">
+        <f>Flows!A16</f>
+        <v>H2</v>
       </c>
       <c r="B16" s="20">
         <v>3364.4250000000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>64</v>
+      <c r="A17" s="6" t="str">
+        <f>Flows!A17</f>
+        <v>B16</v>
       </c>
       <c r="B17" s="20">
         <v>712</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>65</v>
+      <c r="A18" s="6" t="str">
+        <f>Flows!A18</f>
+        <v>B17</v>
       </c>
       <c r="B18" s="20">
         <f>611+126.2</f>
@@ -4611,56 +5201,63 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>66</v>
+      <c r="A19" s="6" t="str">
+        <f>Flows!A19</f>
+        <v>NaOH</v>
       </c>
       <c r="B19" s="20">
         <v>1190</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>67</v>
+      <c r="A20" s="6" t="str">
+        <f>Flows!A20</f>
+        <v>B19</v>
       </c>
       <c r="B20" s="20">
         <v>38.31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>68</v>
+      <c r="A21" s="6" t="str">
+        <f>Flows!A21</f>
+        <v>B20</v>
       </c>
       <c r="B21" s="20">
         <v>28.562999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>69</v>
+      <c r="A22" s="6" t="str">
+        <f>Flows!A22</f>
+        <v>Cl2</v>
       </c>
       <c r="B22" s="20">
         <v>1740</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>70</v>
+      <c r="A23" s="6" t="str">
+        <f>Flows!A23</f>
+        <v>R22</v>
       </c>
       <c r="B23" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>71</v>
+      <c r="A24" s="6" t="str">
+        <f>Flows!A24</f>
+        <v>R23</v>
       </c>
       <c r="B24" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>72</v>
+      <c r="A25" s="6" t="str">
+        <f>Flows!A25</f>
+        <v>R24</v>
       </c>
       <c r="B25" s="20">
         <f>B18</f>
@@ -4668,8 +5265,9 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>73</v>
+      <c r="A26" s="6" t="str">
+        <f>Flows!A26</f>
+        <v>R25</v>
       </c>
       <c r="B26" s="20">
         <f>B21</f>
@@ -4783,13 +5381,13 @@
         <v>47</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4803,12 +5401,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -4817,12 +5415,12 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -4831,12 +5429,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -4845,12 +5443,12 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -4859,12 +5457,12 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -4873,7 +5471,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -4886,7 +5484,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4899,12 +5497,12 @@
         <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -4915,7 +5513,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -4926,7 +5524,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -4937,13 +5535,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -4952,6 +5550,40 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90417662-6BAC-4C8E-825D-9911DD15A77C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:YY34"/>
   <sheetViews>
@@ -4969,7 +5601,7 @@
         <v>48</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -9061,7 +9693,7 @@
     </row>
     <row r="7" spans="1:675" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>35</v>
@@ -9072,7 +9704,7 @@
     </row>
     <row r="8" spans="1:675" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>35</v>
@@ -12776,567 +13408,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AD30"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="18" max="18" width="10.140625" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="16">
-        <v>244</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="16">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="T1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1.2E-2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="17">
-        <f>L2*1000*VLOOKUP(K2,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K2,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>4.6981132075471699</v>
-      </c>
-      <c r="O2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2">
-        <v>23</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB2" s="19">
-        <f>Z2*VLOOKUP(Y2,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(Y2,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>38.3098878695209</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="17">
-        <f>L3*1000*VLOOKUP(K3,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K3,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>5.43025</v>
-      </c>
-      <c r="O3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="1">
-        <f>0.028*0.32</f>
-        <v>8.9600000000000009E-3</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="17">
-        <f>L4*1000*VLOOKUP(K4,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(K4,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>20.74301369863014</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="16">
-        <v>432</v>
-      </c>
-      <c r="P5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" t="s">
-        <v>24</v>
-      </c>
-      <c r="U5" s="16">
-        <f>1787496/1000</f>
-        <v>1787.4960000000001</v>
-      </c>
-      <c r="V5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="16">
-        <f>B7*1000*VLOOKUP(A7,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(A7,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>490.06863449691997</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="16">
-        <f>H7*1000*VLOOKUP(G7,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(G7,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>490.06863449691997</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6">
-        <f>0.911*1.94</f>
-        <v>1.7673399999999999</v>
-      </c>
-      <c r="P6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
-      <c r="V6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <f>0.867*2.31</f>
-        <v>2.0027699999999999</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <f>0.867*2.31</f>
-        <v>2.0027699999999999</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA7">
-        <v>28</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8">
-        <f>2.02+O6*3</f>
-        <v>7.3220200000000002</v>
-      </c>
-      <c r="P8" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
-        <v>8</v>
-      </c>
-      <c r="U8">
-        <f>7.24/91.4*1000</f>
-        <v>79.212253829321668</v>
-      </c>
-      <c r="V8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <f>O8+L13/1000</f>
-        <v>7.8830200000000001</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="16">
-        <f>28563/1000</f>
-        <v>28.562999999999999</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="T10" t="s">
-        <v>24</v>
-      </c>
-      <c r="U10" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="16">
-        <f>B9*1000*VLOOKUP(A9,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(A7,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>12.012320328542096</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="N12" t="s">
-        <v>24</v>
-      </c>
-      <c r="O12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13">
-        <v>561</v>
-      </c>
-      <c r="M13" t="s">
-        <v>4</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="17">
-        <f>1231383/1000</f>
-        <v>1231.383</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R13" t="s">
-        <v>10</v>
-      </c>
-      <c r="S13">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="T13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="16">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>26</v>
-      </c>
-      <c r="R14" t="s">
-        <v>8</v>
-      </c>
-      <c r="S14">
-        <f>S13*2</f>
-        <v>2.2559999999999998</v>
-      </c>
-      <c r="T14" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" t="s">
-        <v>24</v>
-      </c>
-      <c r="W14" s="16">
-        <f>W15*VLOOKUP(V15,Exergías!$A$1:$C$9,2,FALSE)/VLOOKUP(V15,Exergías!$A$1:$C$9,3,FALSE)</f>
-        <v>3364.4249999999997</v>
-      </c>
-      <c r="X14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="V15" t="s">
-        <v>3</v>
-      </c>
-      <c r="W15">
-        <v>28.5</v>
-      </c>
-      <c r="X15" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>1</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="17">
-        <f>AA15*1000*VLOOKUP(Z15,Exergías!$A$1:$C$8,2,FALSE)/VLOOKUP(Z15,Exergías!$A$1:$C$8,3,FALSE)</f>
-        <v>1743.3004231311704</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="O17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="T18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="N19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O19" t="s">
-        <v>14</v>
-      </c>
-      <c r="T19" t="s">
-        <v>2</v>
-      </c>
-      <c r="U19">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="V19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="N20" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20">
-        <v>0.8</v>
-      </c>
-      <c r="P20" t="s">
-        <v>1</v>
-      </c>
-      <c r="T20" t="s">
-        <v>8</v>
-      </c>
-      <c r="U20">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="V20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="AA21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB21" s="1">
-        <f>U22+W14+AC15</f>
-        <v>6302.2324231311704</v>
-      </c>
-    </row>
-    <row r="22" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="N22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O22" s="18">
-        <v>712.15700000000004</v>
-      </c>
-      <c r="P22" t="s">
-        <v>17</v>
-      </c>
-      <c r="T22" t="s">
-        <v>24</v>
-      </c>
-      <c r="U22" s="17">
-        <f>1194507/1000</f>
-        <v>1194.5070000000001</v>
-      </c>
-      <c r="V22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="R25" t="s">
-        <v>12</v>
-      </c>
-      <c r="S25">
-        <f>S14-U20</f>
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="T25" t="s">
-        <v>1</v>
-      </c>
-      <c r="U25" s="19">
-        <v>611</v>
-      </c>
-      <c r="V25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="R26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="R27" t="s">
-        <v>8</v>
-      </c>
-      <c r="S27">
-        <v>0.7</v>
-      </c>
-      <c r="T27" t="s">
-        <v>1</v>
-      </c>
-      <c r="U27" s="16">
-        <v>126.2</v>
-      </c>
-      <c r="V27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="R28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="14:28" x14ac:dyDescent="0.25">
-      <c r="O30" s="1">
-        <f>O22+P13</f>
-        <v>1943.54</v>
-      </c>
-      <c r="P30">
-        <f>U25+U27+U22</f>
-        <v>1931.7070000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="P6">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{EDC1F62B-33C6-4008-932E-86963BF76F55}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EDC1F62B-33C6-4008-932E-86963BF76F55}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>P6</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>